<commit_message>
Fin de l'affichage du score et plus...
</commit_message>
<xml_diff>
--- a/documentation/Journal de bord.xlsx
+++ b/documentation/Journal de bord.xlsx
@@ -1,31 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eliott.JAQUIER\MA20\BatailleNavale\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CPNV\BatailleNavale\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7737F364-3BAE-46BA-8AE8-79358303E535}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5115" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-28920" yWindow="5115" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de bord" sheetId="3" r:id="rId1"/>
     <sheet name="Aide (Référence)" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>De</t>
   </si>
@@ -73,12 +80,33 @@
   </si>
   <si>
     <t>https://www.holbertonschool.com/coding-resource-strcat-in-c</t>
+  </si>
+  <si>
+    <t>https://www.deepl.com/</t>
+  </si>
+  <si>
+    <t>http://source-code-share.blogspot.com/2014/07/implementation-of-java-stringsplit.html</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/50562192/process-finished-with-exit-code-1073740791-0xc0000409-pycharm-error</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/14386/fopen-deprecated-warning</t>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/taking-string-input-space-c-3-different-methods/</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/12306591/read-no-more-than-size-of-string-with-scanf</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/1442116/how-to-get-the-date-and-time-values-in-a-c-program</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -411,7 +439,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -455,11 +483,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,22 +560,64 @@
         <v>15</v>
       </c>
     </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A11" r:id="rId10"/>
-    <hyperlink ref="A12" r:id="rId11"/>
-    <hyperlink ref="A13" r:id="rId12"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="A14" r:id="rId13" xr:uid="{75C4804F-4A44-4D26-8E8F-4A799B7FD260}"/>
+    <hyperlink ref="A15" r:id="rId14" xr:uid="{A22352D4-E177-456B-8C3C-30009B42CA74}"/>
+    <hyperlink ref="A16" r:id="rId15" xr:uid="{568F08B7-2B3C-4FA5-B56A-0BD3EABBBB47}"/>
+    <hyperlink ref="A17" r:id="rId16" xr:uid="{0AB5ADDD-F9A0-4488-9FC2-E1D5B3C77AAB}"/>
+    <hyperlink ref="A18" r:id="rId17" xr:uid="{8B02233F-486F-49D1-B358-E502439748CB}"/>
+    <hyperlink ref="A19" r:id="rId18" xr:uid="{3C3141A6-4F51-4F3D-9C38-978E37D6438A}"/>
+    <hyperlink ref="A20" r:id="rId19" xr:uid="{BC50943F-9608-4FAA-AC4A-0B96F5624FE0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fin du sprint 3, Version 0.1 TERMINEE
</commit_message>
<xml_diff>
--- a/documentation/Journal de bord.xlsx
+++ b/documentation/Journal de bord.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eliott.JAQUIER\MA20\BatailleNavale\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CPNV\BatailleNavale\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672FEA5D-B230-49EB-AE84-AC49780C5374}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5115" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de bord" sheetId="3" r:id="rId1"/>
@@ -19,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>à</t>
   </si>
@@ -69,12 +64,18 @@
   </si>
   <si>
     <t>Fin de l'implémentation de l'affichage des scores</t>
+  </si>
+  <si>
+    <t>Fin du code complet de la Release 0.1</t>
+  </si>
+  <si>
+    <t>Commit de la 0.1 sur GitHub</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -127,13 +128,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,11 +417,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,6 +560,28 @@
         <v>12</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>43908</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>43908</v>
+      </c>
+      <c r="B14" s="7">
+        <v>0.94236111111111109</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajout d'un système de logs
</commit_message>
<xml_diff>
--- a/documentation/Journal de bord.xlsx
+++ b/documentation/Journal de bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CPNV\BatailleNavale\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672FEA5D-B230-49EB-AE84-AC49780C5374}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0437E055-BFB9-4F30-9BAD-1F8A7E989904}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>à</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Commit de la 0.1 sur GitHub</t>
+  </si>
+  <si>
+    <t>Conférence avec Mr. Favre à propos du SPRINT 4</t>
   </si>
 </sst>
 </file>
@@ -128,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -138,6 +141,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,6 +586,17 @@
         <v>14</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>43913</v>
+      </c>
+      <c r="B15" s="9">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajout d'un nouveau système de son (seulement por windows) + de nouveaux graphiques
</commit_message>
<xml_diff>
--- a/documentation/Journal de bord.xlsx
+++ b/documentation/Journal de bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CPNV\BatailleNavale\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0437E055-BFB9-4F30-9BAD-1F8A7E989904}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC4C29C-3884-48E3-B295-19EA1A91374D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>à</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Conférence avec Mr. Favre à propos du SPRINT 4</t>
+  </si>
+  <si>
+    <t>Initiation aux tests fonctionnels</t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,6 +600,17 @@
         <v>15</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>43916</v>
+      </c>
+      <c r="B16" s="9">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajout d'un système de paramètres
</commit_message>
<xml_diff>
--- a/documentation/Journal de bord.xlsx
+++ b/documentation/Journal de bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CPNV\BatailleNavale\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC4C29C-3884-48E3-B295-19EA1A91374D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A0C1C9-210D-4123-BF4C-6735579949AF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>à</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Initiation aux tests fonctionnels</t>
+  </si>
+  <si>
+    <t>Fin du système de sons, images et animations (avec les paramètres associés)</t>
   </si>
 </sst>
 </file>
@@ -107,7 +110,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -130,11 +133,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -145,6 +159,9 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,16 +442,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="3" max="3" width="61.7109375" customWidth="1"/>
+    <col min="3" max="3" width="74.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -611,6 +628,17 @@
         <v>16</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>44012</v>
+      </c>
+      <c r="B17" s="11">
+        <v>21.13</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Restructuration générale du projet GitHub
</commit_message>
<xml_diff>
--- a/documentation/Journal de bord.xlsx
+++ b/documentation/Journal de bord.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CPNV\BatailleNavale\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CPNV\BatailleNavale\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D20FC8-97D3-432E-9597-179BDE0A7F33}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84120BCD-8604-47DC-9B50-29DFB6597636}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="2205" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de bord" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>à</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Ajout d'un animal vertébré aquatique à branchies</t>
+  </si>
+  <si>
+    <t>Fin d'ajouts de fonctionnalités dans l'application pour se concentrer uniquements sur la rectification de bugs et de documentation</t>
   </si>
 </sst>
 </file>
@@ -119,7 +122,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -142,22 +145,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -168,13 +160,11 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,16 +445,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="3" max="3" width="74.5703125" customWidth="1"/>
+    <col min="3" max="3" width="118.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -642,25 +632,36 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
+      <c r="A17" s="6">
         <v>44012</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="10">
         <v>21.13</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+      <c r="A18" s="6">
         <v>43922</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="9">
         <v>0.51180555555555551</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="11" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>43923</v>
+      </c>
+      <c r="B19" s="10">
+        <v>0.39166666666666666</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Suite de la documentation (dossier de projet)
</commit_message>
<xml_diff>
--- a/documentation/Journal de bord.xlsx
+++ b/documentation/Journal de bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CPNV\BatailleNavale\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84120BCD-8604-47DC-9B50-29DFB6597636}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFDAD2A-ECD2-42F2-AEC7-DB0AA38A801C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
-    <t>à</t>
-  </si>
-  <si>
     <t>Initiation à la" planification en mode AGILE par M.Favre"</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>Fin d'ajouts de fonctionnalités dans l'application pour se concentrer uniquements sur la rectification de bugs et de documentation</t>
+  </si>
+  <si>
+    <t>Evenement</t>
   </si>
 </sst>
 </file>
@@ -149,18 +149,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -445,223 +440,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="3" max="3" width="118.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="118.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>43887</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>43887</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>43889</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>43889</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1.03</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>4.03</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>4.03</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>5.03</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>6.03</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>43901</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>43887</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0.45624999999999999</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>43887</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0.49652777777777773</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>43889</v>
-      </c>
-      <c r="B4" s="4">
-        <v>0.59791666666666665</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>43889</v>
-      </c>
-      <c r="B5" s="4">
-        <v>0.59791666666666665</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>1.03</v>
-      </c>
-      <c r="B6" s="4">
-        <v>0.3972222222222222</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>4.03</v>
-      </c>
-      <c r="B7" s="4">
-        <v>0.48194444444444445</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>4.03</v>
-      </c>
-      <c r="B8" s="4">
-        <v>0.48194444444444445</v>
-      </c>
-      <c r="C8" s="5" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>43902.883228125</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>5.03</v>
-      </c>
-      <c r="B9" s="4">
-        <v>0.70486111111111116</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="B10" s="4">
-        <v>0.99930555555555556</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>43901</v>
-      </c>
-      <c r="B11" s="4">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>43902.883228125</v>
-      </c>
-      <c r="B12" s="4">
-        <v>0.99513888888888891</v>
-      </c>
-      <c r="C12" s="5" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>43908</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>43908</v>
       </c>
-      <c r="B13" s="7">
-        <v>0.93055555555555547</v>
-      </c>
-      <c r="C13" s="8" t="s">
+      <c r="B14" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>43908</v>
-      </c>
-      <c r="B14" s="7">
-        <v>0.94236111111111109</v>
-      </c>
-      <c r="C14" s="8" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>43913</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <v>43913</v>
-      </c>
-      <c r="B15" s="9">
-        <v>0.68055555555555547</v>
-      </c>
-      <c r="C15" s="8" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>43916</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
-        <v>43916</v>
-      </c>
-      <c r="B16" s="9">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C16" s="8" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>44012</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <v>44012</v>
-      </c>
-      <c r="B17" s="10">
-        <v>21.13</v>
-      </c>
-      <c r="C17" s="8" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>43922</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <v>43922</v>
-      </c>
-      <c r="B18" s="9">
-        <v>0.51180555555555551</v>
-      </c>
-      <c r="C18" s="11" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>43923</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
-        <v>43923</v>
-      </c>
-      <c r="B19" s="10">
-        <v>0.39166666666666666</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Suite de la documentation et Ajout de la planification initiale
</commit_message>
<xml_diff>
--- a/documentation/Journal de bord.xlsx
+++ b/documentation/Journal de bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CPNV\BatailleNavale\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFDAD2A-ECD2-42F2-AEC7-DB0AA38A801C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6EF657-6F7D-4293-AF9A-850C19B14D80}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -443,7 +443,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
V1.0 Réctifications de bugs, ajout d'une version pre.compilée,modification de la documentation et plus
</commit_message>
<xml_diff>
--- a/documentation/Journal de bord.xlsx
+++ b/documentation/Journal de bord.xlsx
@@ -8,24 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CPNV\BatailleNavale\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6EF657-6F7D-4293-AF9A-850C19B14D80}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05CB7C6-324B-4BE6-B98D-8730B22CB74F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de bord" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Initiation à la" planification en mode AGILE par M.Favre"</t>
   </si>
@@ -85,6 +91,9 @@
   </si>
   <si>
     <t>Evenement</t>
+  </si>
+  <si>
+    <t>Finalisation du projet, export, build et envoy de la 1.0 sur GitHub</t>
   </si>
 </sst>
 </file>
@@ -440,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,6 +613,14 @@
         <v>18</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>43929</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>